<commit_message>
'80% complete report - need to add PCA and final decision tree'
</commit_message>
<xml_diff>
--- a/COSC 528/Project 3/Tables.xlsx
+++ b/COSC 528/Project 3/Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IAN\Research\COSC 528\Project 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i6o/Research/COSC 528/Project 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2E20ADB9-715B-4F1B-BD8D-704894EE7EBE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4247FC1-3E2F-6B4F-86FC-C97BAB67BD79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C6838D18-D074-4A85-BB7E-E639AA8AEA5A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12220" activeTab="1" xr2:uid="{C6838D18-D074-4A85-BB7E-E639AA8AEA5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Confusion Matrices" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="22">
   <si>
     <t>Confusion Matrix for 2-NN</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>F1 Score</t>
+  </si>
+  <si>
+    <t>Training Accuracy</t>
+  </si>
+  <si>
+    <t>Test Accuracy</t>
+  </si>
+  <si>
+    <t>DT Depth</t>
   </si>
 </sst>
 </file>
@@ -90,9 +99,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +122,19 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -322,18 +344,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -382,13 +395,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -398,10 +411,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -720,405 +751,415 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A96835-86A9-42D3-9AFD-730063000327}">
   <dimension ref="A2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="E2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="28"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="15">
+      <c r="F4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12">
         <v>219</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="E5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="12">
         <v>218</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="16">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13">
         <v>9</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="14">
         <v>108</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="16">
-        <v>3</v>
-      </c>
-      <c r="G6" s="17">
+      <c r="E6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="13">
+        <v>3</v>
+      </c>
+      <c r="G6" s="14">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="E8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="28"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="G9" s="28"/>
+    </row>
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="B10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="15">
+      <c r="F10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="12">
         <v>219</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="2">
         <v>5</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="15">
+      <c r="E11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="12">
         <v>218</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="16">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="13">
         <v>5</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="14">
         <v>112</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="16">
+      <c r="E12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="13">
         <v>6</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="14">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="E14" s="2" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="E14" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="28"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="15">
+      <c r="F16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="12">
         <v>219</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="2">
         <v>5</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="15">
+      <c r="E17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="12">
         <v>218</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="16">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="13">
         <v>9</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="14">
         <v>108</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="16">
+      <c r="E18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="13">
         <v>6</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="14">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="E20" s="2" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="E20" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="28"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="B22" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="11">
+      <c r="F22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="8">
         <v>219</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="9">
         <v>6</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="15">
+      <c r="E23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="12">
         <v>219</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="13">
-        <v>3</v>
-      </c>
-      <c r="C24" s="14">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="10">
+        <v>3</v>
+      </c>
+      <c r="C24" s="11">
         <v>114</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="16">
+      <c r="E24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="13">
         <v>8</v>
       </c>
-      <c r="G24" s="17">
+      <c r="G24" s="14">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="C27" s="28"/>
+    </row>
+    <row r="28" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="11">
+      <c r="B28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="8">
         <v>218</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="9">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="13">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="10">
         <v>5</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="11">
         <v>112</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A26:C26"/>
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="E2:G2"/>
@@ -1127,16 +1168,6 @@
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1145,220 +1176,271 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F42810-F889-4908-AD00-82A5204C91A7}">
-  <dimension ref="A2:F14"/>
+  <dimension ref="A2:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H3:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
-        <v>2</v>
-      </c>
-      <c r="B3" s="27">
+      <c r="H2" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24">
         <v>0.96479999999999999</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="18">
         <v>0.94869999999999999</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="24">
         <v>0.94869999999999999</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="18">
         <v>0.97319999999999995</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="24">
         <v>0.94869999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
-        <v>3</v>
-      </c>
-      <c r="B4" s="27">
+      <c r="H3" s="29">
+        <v>2</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+    </row>
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24">
         <v>0.95889999999999997</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>0.92310000000000003</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="24">
         <v>0.95579999999999998</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="18">
         <v>0.97770000000000001</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="24">
         <v>0.93910000000000005</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="H4" s="29">
+        <v>3</v>
+      </c>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+    </row>
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="24">
         <v>0.97070000000000001</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>0.95730000000000004</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="24">
         <v>0.95730000000000004</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="18">
         <v>0.97770000000000001</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="24">
         <v>0.95730000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="H5" s="29">
+        <v>4</v>
+      </c>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="24">
         <v>0.95889999999999997</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>0.92310000000000003</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="24">
         <v>0.95579999999999998</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="18">
         <v>0.97770000000000001</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="24">
         <v>0.93910000000000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="H6" s="29">
+        <v>5</v>
+      </c>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="24">
         <v>0.97360000000000002</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>0.97440000000000004</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="24">
         <v>0.95</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="18">
         <v>0.97319999999999995</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="24">
         <v>0.96199999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="H7" s="29">
+        <v>6</v>
+      </c>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+    </row>
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="24">
         <v>0.9677</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>0.95730000000000004</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="24">
         <v>0.94920000000000004</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="18">
         <v>0.97319999999999995</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="24">
         <v>0.95320000000000005</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="H8" s="29">
+        <v>7</v>
+      </c>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+    </row>
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="24">
         <v>0.97360000000000002</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="18">
         <v>0.97440000000000004</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="24">
         <v>0.95</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="18">
         <v>0.97319999999999995</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="24">
         <v>0.96199999999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
+      <c r="H9" s="30">
+        <v>8</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="J9" s="33">
+        <v>0.86899999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="17">
         <v>17</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="24">
         <v>0.96479999999999999</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>0.94869999999999999</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="24">
         <v>0.94869999999999999</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="18">
         <v>0.97319999999999995</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="24">
         <v>0.94869999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="19">
         <v>33</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="25">
         <v>0.96479999999999999</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="20">
         <v>0.94869999999999999</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="25">
         <v>0.94869999999999999</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="20">
         <v>0.97319999999999995</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="25">
         <v>0.94869999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
'pushing final cosc528 proj3 to master'
</commit_message>
<xml_diff>
--- a/COSC 528/Project 3/Tables.xlsx
+++ b/COSC 528/Project 3/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i6o/Research/COSC 528/Project 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4247FC1-3E2F-6B4F-86FC-C97BAB67BD79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D39F7D5-C447-0042-BB71-059FBA872019}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12220" activeTab="1" xr2:uid="{C6838D18-D074-4A85-BB7E-E639AA8AEA5A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Confusion Matrices" sheetId="1" r:id="rId1"/>
     <sheet name="Performance Metrics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="28">
   <si>
     <t>Confusion Matrix for 2-NN</t>
   </si>
@@ -92,16 +92,35 @@
   </si>
   <si>
     <t>DT Depth</t>
+  </si>
+  <si>
+    <t>Gini index</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Dec. Tree Depth</t>
+  </si>
+  <si>
+    <t>Total Variance Explained</t>
+  </si>
+  <si>
+    <t>PC Variance</t>
+  </si>
+  <si>
+    <t>PC No.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="174" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +154,11 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Var(--jp-code-font-family)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -340,11 +364,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -426,15 +463,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,7 +839,7 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.1640625" customWidth="1"/>
@@ -765,7 +849,7 @@
     <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
@@ -777,7 +861,7 @@
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1"/>
       <c r="B3" s="27" t="s">
         <v>4</v>
@@ -789,7 +873,7 @@
       </c>
       <c r="G3" s="28"/>
     </row>
-    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -809,7 +893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15" customHeight="1" thickTop="1">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -829,7 +913,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -849,7 +933,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="26" t="s">
         <v>5</v>
       </c>
@@ -861,7 +945,7 @@
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" s="27" t="s">
         <v>4</v>
@@ -873,7 +957,7 @@
       </c>
       <c r="G9" s="28"/>
     </row>
-    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -893,7 +977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="16" thickTop="1">
       <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
@@ -913,7 +997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="7" t="s">
         <v>3</v>
       </c>
@@ -933,7 +1017,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="26" t="s">
         <v>6</v>
       </c>
@@ -945,7 +1029,7 @@
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="1"/>
       <c r="B15" s="27" t="s">
         <v>4</v>
@@ -957,7 +1041,7 @@
       </c>
       <c r="G15" s="28"/>
     </row>
-    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -977,7 +1061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="16" thickTop="1">
       <c r="A17" s="6" t="s">
         <v>2</v>
       </c>
@@ -997,7 +1081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="7" t="s">
         <v>3</v>
       </c>
@@ -1017,7 +1101,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="26" t="s">
         <v>7</v>
       </c>
@@ -1029,7 +1113,7 @@
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1"/>
       <c r="B21" s="27" t="s">
         <v>4</v>
@@ -1041,7 +1125,7 @@
       </c>
       <c r="G21" s="28"/>
     </row>
-    <row r="22" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="16" thickBot="1">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -1061,7 +1145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="16" thickTop="1">
       <c r="A23" s="6" t="s">
         <v>2</v>
       </c>
@@ -1081,7 +1165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="7" t="s">
         <v>3</v>
       </c>
@@ -1101,21 +1185,21 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="1"/>
       <c r="B27" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="28"/>
     </row>
-    <row r="28" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="16" thickBot="1">
       <c r="A28" s="3" t="s">
         <v>1</v>
       </c>
@@ -1126,7 +1210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="16" thickTop="1">
       <c r="A29" s="6" t="s">
         <v>2</v>
       </c>
@@ -1137,7 +1221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" s="7" t="s">
         <v>3</v>
       </c>
@@ -1176,13 +1260,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F42810-F889-4908-AD00-82A5204C91A7}">
-  <dimension ref="A2:J14"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H3:H9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
@@ -1190,9 +1274,22 @@
     <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
     <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="17" thickBot="1">
       <c r="A2" s="21" t="s">
         <v>13</v>
       </c>
@@ -1211,17 +1308,35 @@
       <c r="F2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="M2" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="N2" s="50" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="P2" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="17" thickTop="1">
       <c r="A3" s="17">
         <v>2</v>
       </c>
@@ -1243,10 +1358,33 @@
       <c r="H3" s="29">
         <v>2</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-    </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="I3" s="42">
+        <v>0.97076023391812805</v>
+      </c>
+      <c r="J3" s="43">
+        <v>0.96480938416422202</v>
+      </c>
+      <c r="L3" s="34">
+        <v>2</v>
+      </c>
+      <c r="M3" s="36">
+        <v>0.97076023391812805</v>
+      </c>
+      <c r="N3" s="48">
+        <v>0.96480938416422202</v>
+      </c>
+      <c r="P3" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="55">
+        <f>R3</f>
+        <v>59.05</v>
+      </c>
+      <c r="R3" s="53">
+        <v>59.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="16">
       <c r="A4" s="17">
         <v>3</v>
       </c>
@@ -1265,13 +1403,36 @@
       <c r="F4" s="24">
         <v>0.93910000000000005</v>
       </c>
-      <c r="H4" s="29">
-        <v>3</v>
-      </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-    </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="H4" s="30">
+        <v>3</v>
+      </c>
+      <c r="I4" s="44">
+        <v>0.97953216374269003</v>
+      </c>
+      <c r="J4" s="36">
+        <v>0.97067448680351898</v>
+      </c>
+      <c r="L4" s="34">
+        <v>3</v>
+      </c>
+      <c r="M4" s="36">
+        <v>0.97953216374269003</v>
+      </c>
+      <c r="N4" s="48">
+        <v>0.97067448680351898</v>
+      </c>
+      <c r="P4" s="30">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="55">
+        <f>R4-R3</f>
+        <v>10</v>
+      </c>
+      <c r="R4" s="53">
+        <v>69.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="16">
       <c r="A5" s="17">
         <v>4</v>
       </c>
@@ -1290,13 +1451,36 @@
       <c r="F5" s="24">
         <v>0.95730000000000004</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="30">
         <v>4</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-    </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="I5" s="44">
+        <v>0.98245614035087703</v>
+      </c>
+      <c r="J5" s="36">
+        <v>0.96480938416422202</v>
+      </c>
+      <c r="L5" s="34">
+        <v>4</v>
+      </c>
+      <c r="M5" s="36">
+        <v>0.98245614035087703</v>
+      </c>
+      <c r="N5" s="48">
+        <v>0.96480938416422202</v>
+      </c>
+      <c r="P5" s="30">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="55">
+        <f>R5-R4</f>
+        <v>7.75</v>
+      </c>
+      <c r="R5" s="53">
+        <v>76.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="16">
       <c r="A6" s="17">
         <v>5</v>
       </c>
@@ -1315,13 +1499,36 @@
       <c r="F6" s="24">
         <v>0.93910000000000005</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="30">
         <v>5</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-    </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="I6" s="44">
+        <v>0.98538011695906402</v>
+      </c>
+      <c r="J6" s="36">
+        <v>0.96480938416422202</v>
+      </c>
+      <c r="L6" s="34">
+        <v>5</v>
+      </c>
+      <c r="M6" s="36">
+        <v>0.98538011695906402</v>
+      </c>
+      <c r="N6" s="48">
+        <v>0.96480938416422202</v>
+      </c>
+      <c r="P6" s="30">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="55">
+        <f>R6-R5</f>
+        <v>5.4000000000000057</v>
+      </c>
+      <c r="R6" s="53">
+        <v>82.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="16">
       <c r="A7" s="17">
         <v>6</v>
       </c>
@@ -1340,13 +1547,36 @@
       <c r="F7" s="24">
         <v>0.96199999999999997</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="30">
         <v>6</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-    </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="I7" s="44">
+        <v>0.99415204678362501</v>
+      </c>
+      <c r="J7" s="36">
+        <v>0.95894428152492595</v>
+      </c>
+      <c r="L7" s="34">
+        <v>6</v>
+      </c>
+      <c r="M7" s="36">
+        <v>0.98538011695906402</v>
+      </c>
+      <c r="N7" s="48">
+        <v>0.96480938416422202</v>
+      </c>
+      <c r="P7" s="30">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="55">
+        <f>R7-R6</f>
+        <v>4.5600000000000023</v>
+      </c>
+      <c r="R7" s="53">
+        <v>86.76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="16">
       <c r="A8" s="17">
         <v>7</v>
       </c>
@@ -1365,13 +1595,36 @@
       <c r="F8" s="24">
         <v>0.95320000000000005</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="30">
         <v>7</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-    </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="I8" s="45">
+        <v>1</v>
+      </c>
+      <c r="J8" s="36">
+        <v>0.96187683284457404</v>
+      </c>
+      <c r="L8" s="34">
+        <v>7</v>
+      </c>
+      <c r="M8" s="36">
+        <v>0.99122807017543801</v>
+      </c>
+      <c r="N8" s="48">
+        <v>0.93841642228738997</v>
+      </c>
+      <c r="P8" s="30">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="55">
+        <f>R8-R7</f>
+        <v>3.7999999999999972</v>
+      </c>
+      <c r="R8" s="53">
+        <v>90.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="16">
       <c r="A9" s="17">
         <v>8</v>
       </c>
@@ -1393,14 +1646,33 @@
       <c r="H9" s="30">
         <v>8</v>
       </c>
-      <c r="I9" s="33">
-        <v>0.90100000000000002</v>
-      </c>
-      <c r="J9" s="33">
-        <v>0.86899999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I9" s="45">
+        <v>1</v>
+      </c>
+      <c r="J9" s="36">
+        <v>0.96187683284457404</v>
+      </c>
+      <c r="L9" s="34">
+        <v>8</v>
+      </c>
+      <c r="M9" s="36">
+        <v>0.99707602339181201</v>
+      </c>
+      <c r="N9" s="48">
+        <v>0.94721407624633402</v>
+      </c>
+      <c r="P9" s="30">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="55">
+        <f>R9-R8</f>
+        <v>3.019999999999996</v>
+      </c>
+      <c r="R9" s="53">
+        <v>93.58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="16">
       <c r="A10" s="17">
         <v>17</v>
       </c>
@@ -1419,8 +1691,36 @@
       <c r="F10" s="24">
         <v>0.94869999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H10" s="30">
+        <v>9</v>
+      </c>
+      <c r="I10" s="46">
+        <v>1</v>
+      </c>
+      <c r="J10" s="36">
+        <v>0.96187683284457404</v>
+      </c>
+      <c r="L10" s="34">
+        <v>9</v>
+      </c>
+      <c r="M10" s="51">
+        <v>1</v>
+      </c>
+      <c r="N10" s="48">
+        <v>0.94721407624633402</v>
+      </c>
+      <c r="P10" s="30">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="55">
+        <f>R10-R9</f>
+        <v>2.9300000000000068</v>
+      </c>
+      <c r="R10" s="53">
+        <v>96.51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="16">
       <c r="A11" s="19">
         <v>33</v>
       </c>
@@ -1439,8 +1739,123 @@
       <c r="F11" s="25">
         <v>0.94869999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="H11" s="30">
+        <v>10</v>
+      </c>
+      <c r="I11" s="46">
+        <v>1</v>
+      </c>
+      <c r="J11" s="36">
+        <v>0.96187683284457404</v>
+      </c>
+      <c r="L11" s="34">
+        <v>10</v>
+      </c>
+      <c r="M11" s="51">
+        <v>1</v>
+      </c>
+      <c r="N11" s="48">
+        <v>0.94721407624633402</v>
+      </c>
+      <c r="P11" s="30">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="55">
+        <f>R11-R10</f>
+        <v>2.6099999999999994</v>
+      </c>
+      <c r="R11" s="53">
+        <v>99.12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="16">
+      <c r="H12" s="30">
+        <v>17</v>
+      </c>
+      <c r="I12" s="45">
+        <v>1</v>
+      </c>
+      <c r="J12" s="36">
+        <v>0.96187683284457404</v>
+      </c>
+      <c r="L12" s="34">
+        <v>17</v>
+      </c>
+      <c r="M12" s="51">
+        <v>1</v>
+      </c>
+      <c r="N12" s="48">
+        <v>0.94721407624633402</v>
+      </c>
+      <c r="P12" s="31">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="56">
+        <f>R12-R11</f>
+        <v>0.87999999999999545</v>
+      </c>
+      <c r="R12" s="54">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="16">
+      <c r="H13" s="31">
+        <v>33</v>
+      </c>
+      <c r="I13" s="47">
+        <v>1</v>
+      </c>
+      <c r="J13" s="37">
+        <v>0.96187683284457404</v>
+      </c>
+      <c r="L13" s="33">
+        <v>33</v>
+      </c>
+      <c r="M13" s="52">
+        <v>1</v>
+      </c>
+      <c r="N13" s="49">
+        <v>0.94721407624633402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="14.25" customHeight="1"/>
+    <row r="17" spans="8:14" ht="17">
+      <c r="H17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+    </row>
+    <row r="18" spans="8:14" ht="17">
+      <c r="H18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+    </row>
+    <row r="19" spans="8:14" ht="17">
+      <c r="L19" s="35"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+    </row>
+    <row r="20" spans="8:14" ht="17">
+      <c r="L20" s="35"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+    </row>
+    <row r="21" spans="8:14" ht="17">
+      <c r="L21" s="35"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+    </row>
+    <row r="22" spans="8:14" ht="17">
+      <c r="L22" s="35"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+    </row>
+    <row r="23" spans="8:14" ht="17">
+      <c r="L23" s="35"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>